<commit_message>
Updated mapping doc for new pages from old
</commit_message>
<xml_diff>
--- a/docs/DublinDashboard_urls_todolist.xlsx
+++ b/docs/DublinDashboard_urls_todolist.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Google Drive/NCG/Tasks/System Architecture/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Liam\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B06F694D-0D70-4DB0-8A2F-7A861727D009}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="-18560" windowWidth="28800" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="57600" windowHeight="24840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
   <si>
     <t>http://www.dublindashboard.ie/</t>
   </si>
@@ -50,9 +51,6 @@
     <t>http://www.dublindashboard.ie/pages/DublinMapped_1</t>
   </si>
   <si>
-    <t>http://www.dublindashboard.ie/pages/DublinPlanning</t>
-  </si>
-  <si>
     <t>http://www.dublindashboard.ie/pages/DublinAccessibility</t>
   </si>
   <si>
@@ -77,9 +75,6 @@
     <t>http://www.dublindashboard.ie/pages/MappedLiveRegister</t>
   </si>
   <si>
-    <t>http://www.dublindashboard.ie/pages/DublinTravel</t>
-  </si>
-  <si>
     <t>http://www.dublindashboard.ie/pages/DublinEnvironment</t>
   </si>
   <si>
@@ -194,9 +189,6 @@
     <t>http://www.dublindashboard.ie/pages/dublin_bay</t>
   </si>
   <si>
-    <t>http://www.dublindashboard.ie/dublindashboard/ScatsMap.html</t>
-  </si>
-  <si>
     <t>http://www.dublindashboard.ie/HealthEducation/stats/</t>
   </si>
   <si>
@@ -225,12 +217,69 @@
   </si>
   <si>
     <t>New Datasource</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.dublindashboard.ie/pages/DublinPlanning </t>
+  </si>
+  <si>
+    <t>SCATs on Map with popup traffic trend data for 7days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.dublindashboard.ie/dublindashboard/ScatsMap.html </t>
+  </si>
+  <si>
+    <t>themes/transport</t>
+  </si>
+  <si>
+    <t>Trend graphs</t>
+  </si>
+  <si>
+    <t>Static housing and/ or planning data</t>
+  </si>
+  <si>
+    <t>/theme/housing or planning? tool/planning ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.dublindashboard.ie/pages/DublinTravel </t>
+  </si>
+  <si>
+    <t>Realtime traffic &amp; travel</t>
+  </si>
+  <si>
+    <t>Map with trend graphs &amp; indicators (Sam)</t>
+  </si>
+  <si>
+    <t>Old top-level page</t>
+  </si>
+  <si>
+    <t>Delete</t>
+  </si>
+  <si>
+    <t>/themes (submenu?)</t>
+  </si>
+  <si>
+    <t>Homepage for Indicators (How's Dublin Doing?)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.dublindashboard.ie/DublinDashboard/home </t>
+  </si>
+  <si>
+    <t>Home page incl links to ext Dublin Bus tc</t>
+  </si>
+  <si>
+    <t>Include external RTPI etc?</t>
+  </si>
+  <si>
+    <t>themes/demographics</t>
+  </si>
+  <si>
+    <t>themes/health</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -287,30 +336,82 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="5" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{DFE5E3A9-1820-445F-9A46-28CB7A5C2E29}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -578,350 +679,523 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="2" width="69.83203125" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" customWidth="1"/>
-    <col min="4" max="4" width="32.83203125" customWidth="1"/>
-    <col min="5" max="5" width="49.5" customWidth="1"/>
-    <col min="6" max="6" width="34.6640625" customWidth="1"/>
-    <col min="7" max="7" width="43.5" customWidth="1"/>
+    <col min="1" max="1" width="24.125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="23.75" style="6" customWidth="1"/>
+    <col min="3" max="3" width="69.875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="25.125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="32.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="34.625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="43.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C8" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="F8" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="9"/>
+    </row>
+    <row r="19" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="9"/>
+    </row>
+    <row r="20" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
+      <c r="C24" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="11"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C50" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C51" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C52" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C54" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C57" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C58" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C60" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C61" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="4"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C65" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C66" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C67" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C68" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C69" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C70" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C71" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C72" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C73" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
+    <row r="74" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C74" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+    <row r="75" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C75" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C76" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="49" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>49</v>
-      </c>
-      <c r="D50" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>56</v>
-      </c>
-    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C24" r:id="rId1" xr:uid="{1110ED4E-8929-4A22-AE74-0A2B3D2C74B9}"/>
+    <hyperlink ref="C23" r:id="rId2" xr:uid="{051A22CE-FBB0-4F0D-9B91-FAC0187B67DD}"/>
+    <hyperlink ref="C8" r:id="rId3" xr:uid="{8D1903BA-49E5-4D19-8899-4DBBF799AC4F}"/>
+    <hyperlink ref="C9" r:id="rId4" xr:uid="{68DF5DDA-8C5C-471B-BE0C-A42EAFD2453B}"/>
+    <hyperlink ref="C11" r:id="rId5" xr:uid="{5D0653CC-FBAD-4D8F-9399-80583FF757FC}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{311E7833-D8CD-41BD-8089-FA383551528B}"/>
+    <hyperlink ref="C5" r:id="rId7" xr:uid="{93DAEA18-BAD2-4376-AFD6-D2278D997C9B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Noted health charts to move
</commit_message>
<xml_diff>
--- a/docs/DublinDashboard_urls_todolist.xlsx
+++ b/docs/DublinDashboard_urls_todolist.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mleigh/Sites/BCD_DD_Versions/bcd-dd-v2/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/losullivan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1443CDC5-0359-4646-8B32-00D921B33121}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="-18980" windowWidth="30620" windowHeight="17200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="109">
   <si>
     <t>http://www.dublindashboard.ie/</t>
   </si>
@@ -350,12 +349,18 @@
   </si>
   <si>
     <t>http://www.failteireland.ie/Research-Insights/Tourism-Facts-and-Figures.aspx</t>
+  </si>
+  <si>
+    <t>trolleys, healthlevels</t>
+  </si>
+  <si>
+    <t>Patients on Trolleys, Health Levels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -477,7 +482,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{DFE5E3A9-1820-445F-9A46-28CB7A5C2E29}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -755,11 +760,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G86"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82:XFD82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1373,46 +1378,52 @@
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C81" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" s="3" t="s">
+      <c r="D81" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C83" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C83" s="3" t="s">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C84" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" s="3" t="s">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C85" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" s="3" t="s">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C86" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C86" s="3" t="s">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C87" s="3" t="s">
         <v>52</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" xr:uid="{1110ED4E-8929-4A22-AE74-0A2B3D2C74B9}"/>
-    <hyperlink ref="C23" r:id="rId2" xr:uid="{051A22CE-FBB0-4F0D-9B91-FAC0187B67DD}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{8D1903BA-49E5-4D19-8899-4DBBF799AC4F}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{68DF5DDA-8C5C-471B-BE0C-A42EAFD2453B}"/>
-    <hyperlink ref="C11" r:id="rId5" xr:uid="{5D0653CC-FBAD-4D8F-9399-80583FF757FC}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{311E7833-D8CD-41BD-8089-FA383551528B}"/>
-    <hyperlink ref="C5" r:id="rId7" xr:uid="{93DAEA18-BAD2-4376-AFD6-D2278D997C9B}"/>
-    <hyperlink ref="C28" r:id="rId8" location="tab1-tab" xr:uid="{39587180-E9BB-0245-989E-2DBD344FDFAB}"/>
+    <hyperlink ref="C24" r:id="rId1"/>
+    <hyperlink ref="C23" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId3"/>
+    <hyperlink ref="C9" r:id="rId4"/>
+    <hyperlink ref="C11" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId7"/>
+    <hyperlink ref="C28" r:id="rId8" location="tab1-tab"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>

</xml_diff>